<commit_message>
Added test for earning points. Meanwages in tb_pens and called by year for earning points.
Former-commit-id: eb7241c3db2b4ab5725c9342562ae9fbcf798ca7
Former-commit-id: 69d6a4e84c5e1a4ba1e1388fe9362a1a0bb9f2aa
</commit_message>
<xml_diff>
--- a/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_pensions.xlsx
+++ b/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_pensions.xlsx
@@ -165,12 +165,13 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="37.64"/>
@@ -525,7 +526,7 @@
         <v>5.9814</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>6.14036992575151</v>
+        <v>6.13401112872145</v>
       </c>
       <c r="O7" s="0" t="n">
         <v>67</v>

</xml_diff>

<commit_message>
Added handcoded test data.
Former-commit-id: 93cab6252496d093627a002a47e327eb173a01b0
Former-commit-id: c5e3c1c2fa7db76e0dfb66431a0ce61fabd77a07
</commit_message>
<xml_diff>
--- a/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_pensions.xlsx
+++ b/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_pensions.xlsx
@@ -164,8 +164,8 @@
   </sheetPr>
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,9 +269,11 @@
         <v>34.9842779743529</v>
       </c>
       <c r="O2" s="0" t="n">
+        <f aca="false">IF(H2&gt;1947, MIN(67, (H2 - 1947) / 12  + 65),  65)</f>
         <v>65.9166666666667</v>
       </c>
       <c r="P2" s="0" t="n">
+        <f aca="false"> (F2 - O2) * 0.036 + 1</f>
         <v>0.679</v>
       </c>
       <c r="Q2" s="0" t="n">
@@ -321,9 +323,11 @@
         <v>36.1021559487058</v>
       </c>
       <c r="O3" s="0" t="n">
+        <f aca="false">IF(H3&gt;1947, MIN(67, (H3 - 1947) / 12  + 65),  65)</f>
         <v>65.8333333333333</v>
       </c>
       <c r="P3" s="0" t="n">
+        <f aca="false"> (F3 - O3) * 0.036 + 1</f>
         <v>0.718</v>
       </c>
       <c r="Q3" s="0" t="n">
@@ -373,9 +377,11 @@
         <v>10.7237339230587</v>
       </c>
       <c r="O4" s="0" t="n">
+        <f aca="false">IF(H4&gt;1947, MIN(67, (H4 - 1947) / 12  + 65),  65)</f>
         <v>67</v>
       </c>
       <c r="P4" s="0" t="n">
+        <f aca="false"> (F4 - O4) * 0.036 + 1</f>
         <v>-0.224</v>
       </c>
       <c r="Q4" s="0" t="n">
@@ -425,9 +431,11 @@
         <v>23.7342118974116</v>
       </c>
       <c r="O5" s="0" t="n">
+        <f aca="false">IF(H5&gt;1947, MIN(67, (H5 - 1947) / 12  + 65),  65)</f>
         <v>66.9166666666667</v>
       </c>
       <c r="P5" s="0" t="n">
+        <f aca="false"> (F5 - O5) * 0.036 + 1</f>
         <v>0.211</v>
       </c>
       <c r="Q5" s="0" t="n">
@@ -477,9 +485,11 @@
         <v>39.4248898717645</v>
       </c>
       <c r="O6" s="0" t="n">
+        <f aca="false">IF(H6&gt;1947, MIN(67, (H6 - 1947) / 12  + 65),  65)</f>
         <v>65.4166666666667</v>
       </c>
       <c r="P6" s="0" t="n">
+        <f aca="false"> (F6 - O6) * 0.036 + 1</f>
         <v>0.913</v>
       </c>
       <c r="Q6" s="0" t="n">
@@ -529,9 +539,11 @@
         <v>6.13401112872145</v>
       </c>
       <c r="O7" s="0" t="n">
+        <f aca="false">IF(H7&gt;1947, MIN(67, (H7 - 1947) / 12  + 65),  65)</f>
         <v>67</v>
       </c>
       <c r="P7" s="0" t="n">
+        <f aca="false"> (F7 - O7) * 0.036 + 1</f>
         <v>-0.44</v>
       </c>
       <c r="Q7" s="0" t="n">
@@ -581,9 +593,11 @@
         <v>8.56673819554509</v>
       </c>
       <c r="O8" s="0" t="n">
+        <f aca="false">IF(H8&gt;1947, MIN(67, (H8 - 1947) / 12  + 65),  65)</f>
         <v>67</v>
       </c>
       <c r="P8" s="0" t="n">
+        <f aca="false"> (F8 - O8) * 0.036 + 1</f>
         <v>-0.332</v>
       </c>
       <c r="Q8" s="0" t="n">
@@ -633,9 +647,11 @@
         <v>18.3025424527289</v>
       </c>
       <c r="O9" s="0" t="n">
+        <f aca="false">IF(H9&gt;1947, MIN(67, (H9 - 1947) / 12  + 65),  65)</f>
         <v>67</v>
       </c>
       <c r="P9" s="0" t="n">
+        <f aca="false"> (F9 - O9) * 0.036 + 1</f>
         <v>-0.00800000000000001</v>
       </c>
       <c r="Q9" s="0" t="n">
@@ -685,9 +701,11 @@
         <v>21.3995136790934</v>
       </c>
       <c r="O10" s="0" t="n">
+        <f aca="false">IF(H10&gt;1947, MIN(67, (H10 - 1947) / 12  + 65),  65)</f>
         <v>66.75</v>
       </c>
       <c r="P10" s="0" t="n">
+        <f aca="false"> (F10 - O10) * 0.036 + 1</f>
         <v>0.109</v>
       </c>
       <c r="Q10" s="0" t="n">
@@ -737,9 +755,11 @@
         <v>25.3882849054578</v>
       </c>
       <c r="O11" s="0" t="n">
+        <f aca="false">IF(H11&gt;1947, MIN(67, (H11 - 1947) / 12  + 65),  65)</f>
         <v>66.4166666666667</v>
       </c>
       <c r="P11" s="0" t="n">
+        <f aca="false"> (F11 - O11) * 0.036 + 1</f>
         <v>0.265</v>
       </c>
       <c r="Q11" s="0" t="n">
@@ -789,9 +809,11 @@
         <v>22.4698561318223</v>
       </c>
       <c r="O12" s="0" t="n">
+        <f aca="false">IF(H12&gt;1947, MIN(67, (H12 - 1947) / 12  + 65),  65)</f>
         <v>66.6666666666667</v>
       </c>
       <c r="P12" s="0" t="n">
+        <f aca="false"> (F12 - O12) * 0.036 + 1</f>
         <v>0.148</v>
       </c>
       <c r="Q12" s="0" t="n">
@@ -841,9 +863,11 @@
         <v>35.3895058166817</v>
       </c>
       <c r="O13" s="0" t="n">
+        <f aca="false">IF(H13&gt;1947, MIN(67, (H13 - 1947) / 12  + 65),  65)</f>
         <v>65.3333333333333</v>
       </c>
       <c r="P13" s="0" t="n">
+        <f aca="false"> (F13 - O13) * 0.036 + 1</f>
         <v>0.772</v>
       </c>
       <c r="Q13" s="0" t="n">
@@ -892,9 +916,11 @@
         <v>30.5848557896052</v>
       </c>
       <c r="O14" s="0" t="n">
+        <f aca="false">IF(H14&gt;1947, MIN(67, (H14 - 1947) / 12  + 65),  65)</f>
         <v>66.0833333333333</v>
       </c>
       <c r="P14" s="0" t="n">
+        <f aca="false"> (F14 - O14) * 0.036 + 1</f>
         <v>0.493</v>
       </c>
       <c r="Q14" s="0" t="n">
@@ -943,9 +969,11 @@
         <v>31.0625</v>
       </c>
       <c r="O15" s="0" t="n">
+        <f aca="false">IF(H15&gt;1947, MIN(67, (H15 - 1947) / 12  + 65),  65)</f>
         <v>66</v>
       </c>
       <c r="P15" s="0" t="n">
+        <f aca="false"> (F15 - O15) * 0.036 + 1</f>
         <v>0.532</v>
       </c>
       <c r="Q15" s="0" t="n">

</xml_diff>